<commit_message>
tambah UI riwayat dosen
</commit_message>
<xml_diff>
--- a/daftar kelompok.xlsx
+++ b/daftar kelompok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FASTIKOM\KULIAH\PEMROGRAMAN FRAMEWORK\2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WWW\aplikasi-portal-dosen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1189,16 +1189,16 @@
     <t>RIWAYAT JABATAN</t>
   </si>
   <si>
-    <t>RIWAYAT PELATIHAN</t>
-  </si>
-  <si>
-    <t>RIWAYAT PENGHARGAAN</t>
-  </si>
-  <si>
     <t>RIWAYAT PUBLIKASI</t>
   </si>
   <si>
     <t>FORM BIODATA</t>
+  </si>
+  <si>
+    <t>RIWAYAT MENGAJAR</t>
+  </si>
+  <si>
+    <t>RIWAYAT SERTIFIKASI</t>
   </si>
 </sst>
 </file>
@@ -2991,7 +2991,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,7 +3043,7 @@
         <v>209</v>
       </c>
       <c r="D5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>217</v>
       </c>
       <c r="D9" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3113,7 +3113,7 @@
         <v>219</v>
       </c>
       <c r="D10" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>221</v>
       </c>
       <c r="D11" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>